<commit_message>
Update diagnostic script by including all tables of interest, export clean diagnostic files to g_intermediate
</commit_message>
<xml_diff>
--- a/p_parameters/additional_concepts.xlsx
+++ b/p_parameters/additional_concepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0334039A-7098-1743-8A1C-1791DD893AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976870E3-454B-3A4D-8AF8-25397A9BCE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>table</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>kg/m2</t>
+  </si>
+  <si>
+    <t>so_unit</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,7 +676,7 @@
         <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="O4" t="s">
         <v>32</v>
@@ -760,7 +763,7 @@
         <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="O7" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Add migraine information to create conceptsets
</commit_message>
<xml_diff>
--- a/p_parameters/additional_concepts.xlsx
+++ b/p_parameters/additional_concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976870E3-454B-3A4D-8AF8-25397A9BCE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C904E6-DEA3-7341-8C07-2A4A054C1F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="58">
   <si>
     <t>table</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>so_unit</t>
+  </si>
+  <si>
+    <t>Migraine_diagnoses</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -934,6 +937,93 @@
         <v>30</v>
       </c>
     </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s">
+        <v>56</v>
+      </c>
+      <c r="O16" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add information from birth registry diagnoses as checkbox for migraine
</commit_message>
<xml_diff>
--- a/p_parameters/additional_concepts.xlsx
+++ b/p_parameters/additional_concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15BFE06-512D-0C42-BC85-912A9C06CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54454211-E73F-284C-A997-2B4E4F13EA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0939CFEC-D1BA-1D42-BACE-55536FF5F5D7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{0939CFEC-D1BA-1D42-BACE-55536FF5F5D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="76">
   <si>
     <t>table</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>Migraine_medicines</t>
+  </si>
+  <si>
+    <t>Migraine_cat_diagnoses</t>
+  </si>
+  <si>
+    <t>MIgraine_medicines</t>
   </si>
 </sst>
 </file>
@@ -280,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -343,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -353,6 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FD393A-5674-3749-B00C-5DA732AD43E3}">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,61 +1020,61 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="C10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="K10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="P10" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="C11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="K11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1072,8 +1085,8 @@
       <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
+      <c r="C12" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>44</v>
@@ -1117,33 +1130,27 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>22</v>
+    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1154,7 +1161,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>44</v>
@@ -1183,7 +1190,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>44</v>
@@ -1206,37 +1213,31 @@
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="2">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1247,19 +1248,19 @@
         <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="G18" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>28</v>
@@ -1285,23 +1286,17 @@
         <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
       </c>
-      <c r="H19" s="2">
-        <v>2</v>
-      </c>
-      <c r="I19" s="2">
-        <v>3</v>
-      </c>
       <c r="K19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1332,11 +1327,17 @@
         <v>26</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
       </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3</v>
+      </c>
       <c r="K20" s="2" t="s">
         <v>28</v>
       </c>
@@ -1361,13 +1362,13 @@
         <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" s="2">
         <v>1</v>
@@ -1387,25 +1388,37 @@
     </row>
     <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1416,7 +1429,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>44</v>
@@ -1431,71 +1444,56 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>22</v>
+    <row r="24" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1</v>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="K25" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1515,7 +1513,7 @@
         <v>26</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
@@ -1544,16 +1542,16 @@
         <v>61</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G27" s="4">
         <v>1</v>
@@ -1591,7 +1589,7 @@
         <v>26</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28" s="4">
         <v>1</v>
@@ -1629,7 +1627,7 @@
         <v>26</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G29" s="4">
         <v>1</v>
@@ -1652,54 +1650,63 @@
     </row>
     <row r="30" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K30" s="3" t="s">
+      <c r="E31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="P30" s="3" t="s">
+      <c r="P31" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1710,7 +1717,7 @@
         <v>58</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>44</v>
@@ -1739,7 +1746,7 @@
         <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>44</v>
@@ -1762,54 +1769,54 @@
     </row>
     <row r="34" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K34" s="5" t="s">
+      <c r="E35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P34" s="5" t="s">
+      <c r="P35" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1820,7 +1827,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>44</v>
@@ -1849,7 +1856,7 @@
         <v>62</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>44</v>
@@ -1872,57 +1879,57 @@
     </row>
     <row r="38" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K38" s="6" t="s">
+      <c r="E39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P38" s="6" t="s">
+      <c r="P39" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:18" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P39" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>16</v>
       </c>
@@ -1930,7 +1937,7 @@
         <v>70</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>44</v>
@@ -1959,7 +1966,7 @@
         <v>70</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>44</v>
@@ -1982,13 +1989,13 @@
     </row>
     <row r="42" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>44</v>
@@ -2000,13 +2007,13 @@
         <v>19</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="P42" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2017,7 +2024,7 @@
         <v>70</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>44</v>
@@ -2046,31 +2053,25 @@
         <v>70</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G44" s="7">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="P44" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R44" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2081,135 +2082,141 @@
         <v>70</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G45" s="7">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="P45" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R45" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="P46" s="7" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="R46" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C47" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K47" s="7" t="s">
+      <c r="E49" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K49" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P47" s="7" t="s">
+      <c r="P49" s="7" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K48" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P48" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K49" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P49" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2220,7 +2227,7 @@
         <v>69</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>44</v>
@@ -2243,84 +2250,60 @@
     </row>
     <row r="51" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="P51" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R51" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M52" s="8" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="P52" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R52" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2331,10 +2314,10 @@
         <v>69</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>44</v>
@@ -2372,10 +2355,10 @@
         <v>69</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>44</v>
@@ -2407,24 +2390,106 @@
     </row>
     <row r="55" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C55" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P55" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R55" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M56" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P56" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R56" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K55" s="8" t="s">
+      <c r="E57" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K57" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="P55" s="8" t="s">
+      <c r="P57" s="8" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add birth registry information for OSLO
</commit_message>
<xml_diff>
--- a/p_parameters/additional_concepts.xlsx
+++ b/p_parameters/additional_concepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/DP4_Migraine_GitHub/Demonstration project/DP4_Migraine/p_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54454211-E73F-284C-A997-2B4E4F13EA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1A28B7-9FC2-D64E-84B2-6FB7EF657525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{0939CFEC-D1BA-1D42-BACE-55536FF5F5D7}"/>
+    <workbookView xWindow="600" yWindow="1600" windowWidth="28800" windowHeight="16380" xr2:uid="{0939CFEC-D1BA-1D42-BACE-55536FF5F5D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="76">
   <si>
     <t>table</t>
   </si>
@@ -681,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FD393A-5674-3749-B00C-5DA732AD43E3}">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,6 +694,7 @@
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.83203125" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -1467,721 +1468,697 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="4">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>29</v>
+    <row r="25" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="4">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="K28" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R28" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="4">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="K29" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" s="4">
-        <v>1</v>
-      </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="K30" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R30" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="3" t="s">
+      <c r="E37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="P37" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+    <row r="38" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K32" s="5" t="s">
+      <c r="E38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P32" s="5" t="s">
+      <c r="P38" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+    <row r="39" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="5" t="s">
+      <c r="E39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P33" s="5" t="s">
+      <c r="P39" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+    <row r="40" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K34" s="5" t="s">
+      <c r="E40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P34" s="5" t="s">
+      <c r="P40" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+    <row r="41" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="5" t="s">
+      <c r="E41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P35" s="5" t="s">
+      <c r="P41" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="42" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="6" t="s">
+      <c r="E43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="L43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P36" s="6" t="s">
+      <c r="P43" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+    <row r="44" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K37" s="6" t="s">
+      <c r="E44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L37" s="6" t="s">
+      <c r="L44" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P37" s="6" t="s">
+      <c r="P44" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+    <row r="45" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K38" s="6" t="s">
+      <c r="E45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L38" s="6" t="s">
+      <c r="L45" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P38" s="6" t="s">
+      <c r="P45" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+    <row r="46" spans="1:18" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="6" t="s">
+      <c r="E46" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K46" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P39" s="6" t="s">
+      <c r="P46" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+    <row r="47" spans="1:18" s="7" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P40" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P41" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P42" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L43" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L44" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="P44" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="P45" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G46" s="7">
-        <v>1</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="P46" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="R46" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G47" s="7">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P47" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="R47" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>44</v>
@@ -2189,307 +2166,545 @@
       <c r="F48" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="G48" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="K48" s="7" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="P48" s="7" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P49" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L50" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P53" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" s="7">
+        <v>1</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P54" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R54" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K49" s="7" t="s">
+      <c r="E56" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P49" s="7" t="s">
+      <c r="P56" s="7" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K50" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P50" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K51" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P51" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K52" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P52" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K53" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M53" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P53" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R53" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K54" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L54" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M54" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P54" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R54" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K55" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M55" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P55" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R55" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K56" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L56" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M56" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P56" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R56" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C57" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P57" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L58" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P58" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P59" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L60" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M60" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P60" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R60" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L61" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P61" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R61" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L62" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M62" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P62" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R62" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L63" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M63" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P63" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R63" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K57" s="8" t="s">
+      <c r="E64" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="P57" s="8" t="s">
+      <c r="P64" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P65" s="8" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merging DP4 PE/GDM/Migraine Algorithm+DU
</commit_message>
<xml_diff>
--- a/p_parameters/additional_concepts.xlsx
+++ b/p_parameters/additional_concepts.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhoxhaj/Desktop/Repositories/DP4_Github/Demonstration project/ConcePTION-DP4_Migraine/p_parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\durable\ConcePTION\DP4\DP4_Migraine_Algorithm\DP4_Migraine_20241225\p_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BF72BE-9F0B-7441-B03F-C6D759EA65D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6296C8C-A9E6-4A7B-9D6F-2F7FB8EBE8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29445" yWindow="4740" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$73</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="124">
   <si>
     <t>table</t>
   </si>
@@ -300,6 +303,114 @@
   </si>
   <si>
     <t>027987066</t>
+  </si>
+  <si>
+    <t>PARITY_checkbox</t>
+  </si>
+  <si>
+    <t>obesity_checkbox</t>
+  </si>
+  <si>
+    <t>blht_checkbox</t>
+  </si>
+  <si>
+    <t>bldm_checkbox</t>
+  </si>
+  <si>
+    <t>obesity_event</t>
+  </si>
+  <si>
+    <t>blht_event</t>
+  </si>
+  <si>
+    <t>bldm_event</t>
+  </si>
+  <si>
+    <t>bldep_event</t>
+  </si>
+  <si>
+    <t>du_medicines</t>
+  </si>
+  <si>
+    <t>PBMI_height</t>
+  </si>
+  <si>
+    <t>PBMI_weight</t>
+  </si>
+  <si>
+    <t>PARITY</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>paritet_5</t>
+  </si>
+  <si>
+    <t>OW</t>
+  </si>
+  <si>
+    <t>kmi_foer</t>
+  </si>
+  <si>
+    <t>BLHT</t>
+  </si>
+  <si>
+    <t>hypertensjon_kronisk</t>
+  </si>
+  <si>
+    <t>BLDM</t>
+  </si>
+  <si>
+    <t>BLOB</t>
+  </si>
+  <si>
+    <t>BLDEP</t>
+  </si>
+  <si>
+    <t>DU_MED</t>
+  </si>
+  <si>
+    <t>PARITE</t>
+  </si>
+  <si>
+    <t>SAIL</t>
+  </si>
+  <si>
+    <t>SERVICE_USER_PARITY_CD</t>
+  </si>
+  <si>
+    <t>PBMI_h</t>
+  </si>
+  <si>
+    <t>SERVICE_USER_HEIGHT</t>
+  </si>
+  <si>
+    <t>PBMI_w</t>
+  </si>
+  <si>
+    <t>SERVICE_USER_WEIGHT_KG</t>
+  </si>
+  <si>
+    <t>EVENT_CD</t>
+  </si>
+  <si>
+    <t>aiemmatsynnytykset</t>
+  </si>
+  <si>
+    <t>apituus</t>
+  </si>
+  <si>
+    <t>apaino</t>
+  </si>
+  <si>
+    <t>PARTI_PR</t>
+  </si>
+  <si>
+    <t>ALTEZZA_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PESO_M </t>
   </si>
 </sst>
 </file>
@@ -720,25 +831,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:R119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,7 +905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -838,7 +949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -882,7 +993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -926,7 +1037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -968,7 +1079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1012,7 +1123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1064,7 +1175,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1108,7 +1219,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1152,7 +1263,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -1192,7 +1303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1232,7 +1343,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -1266,7 +1377,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -1300,7 +1411,7 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -1334,7 +1445,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1368,7 +1479,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1402,7 +1513,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1446,7 +1557,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1490,7 +1601,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1534,7 +1645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +1689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1622,7 +1733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -1666,7 +1777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1710,7 +1821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -1754,7 +1865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
@@ -1794,7 +1905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
@@ -1834,7 +1945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
@@ -1868,7 +1979,7 @@
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
@@ -1902,7 +2013,7 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
@@ -1946,7 +2057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
@@ -1990,7 +2101,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>18</v>
       </c>
@@ -2034,7 +2145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
@@ -2074,7 +2185,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>46</v>
       </c>
@@ -2114,7 +2225,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>46</v>
       </c>
@@ -2148,7 +2259,7 @@
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
     </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>18</v>
       </c>
@@ -2192,7 +2303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>18</v>
       </c>
@@ -2236,7 +2347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>18</v>
       </c>
@@ -2280,7 +2391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>46</v>
       </c>
@@ -2320,7 +2431,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
@@ -2360,7 +2471,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>46</v>
       </c>
@@ -2394,7 +2505,7 @@
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>46</v>
       </c>
@@ -2428,7 +2539,7 @@
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
     </row>
-    <row r="42" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>46</v>
       </c>
@@ -2462,7 +2573,7 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>46</v>
       </c>
@@ -2496,7 +2607,7 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>46</v>
       </c>
@@ -2530,7 +2641,7 @@
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>46</v>
       </c>
@@ -2564,7 +2675,7 @@
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>18</v>
       </c>
@@ -2608,7 +2719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>18</v>
       </c>
@@ -2652,7 +2763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>18</v>
       </c>
@@ -2696,7 +2807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>30</v>
       </c>
@@ -2740,7 +2851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>30</v>
       </c>
@@ -2784,7 +2895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>30</v>
       </c>
@@ -2826,7 +2937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>30</v>
       </c>
@@ -2870,7 +2981,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>30</v>
       </c>
@@ -2914,7 +3025,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>46</v>
       </c>
@@ -2954,7 +3065,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>46</v>
       </c>
@@ -2994,7 +3105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>46</v>
       </c>
@@ -3028,7 +3139,7 @@
       <c r="Q56" s="7"/>
       <c r="R56" s="7"/>
     </row>
-    <row r="57" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>46</v>
       </c>
@@ -3062,7 +3173,7 @@
       <c r="Q57" s="7"/>
       <c r="R57" s="7"/>
     </row>
-    <row r="58" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>18</v>
       </c>
@@ -3106,7 +3217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>18</v>
       </c>
@@ -3150,7 +3261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>18</v>
       </c>
@@ -3194,7 +3305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>30</v>
       </c>
@@ -3238,7 +3349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>30</v>
       </c>
@@ -3282,7 +3393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>46</v>
       </c>
@@ -3322,7 +3433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>46</v>
       </c>
@@ -3362,7 +3473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>46</v>
       </c>
@@ -3402,7 +3513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>46</v>
       </c>
@@ -3442,7 +3553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>46</v>
       </c>
@@ -3482,7 +3593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>46</v>
       </c>
@@ -3522,7 +3633,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>46</v>
       </c>
@@ -3562,7 +3673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>46</v>
       </c>
@@ -3602,7 +3713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>46</v>
       </c>
@@ -3642,7 +3753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>46</v>
       </c>
@@ -3682,7 +3793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>46</v>
       </c>
@@ -3722,58 +3833,1498 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="9"/>
+    <row r="74" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" t="s">
+        <v>88</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
+      <c r="K74" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
+      <c r="P74" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-    </row>
-    <row r="75" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="9"/>
+      <c r="R74" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
+      <c r="K75" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
+      <c r="P75" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-    </row>
-    <row r="76" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="1"/>
+      <c r="R75" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" t="s">
+        <v>90</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1</v>
+      </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
+      <c r="K76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
+      <c r="P76" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" t="s">
+        <v>91</v>
+      </c>
+      <c r="D77" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" t="s">
+        <v>33</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>3</v>
+      </c>
+      <c r="K77" t="s">
+        <v>35</v>
+      </c>
+      <c r="L77" t="s">
+        <v>36</v>
+      </c>
+      <c r="P77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" t="s">
+        <v>107</v>
+      </c>
+      <c r="E78" t="s">
+        <v>22</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G78" t="s">
+        <v>24</v>
+      </c>
+      <c r="K78" t="s">
+        <v>25</v>
+      </c>
+      <c r="L78" t="s">
+        <v>26</v>
+      </c>
+      <c r="P78" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>93</v>
+      </c>
+      <c r="D79" t="s">
+        <v>104</v>
+      </c>
+      <c r="E79" t="s">
+        <v>22</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G79" t="s">
+        <v>24</v>
+      </c>
+      <c r="K79" t="s">
+        <v>25</v>
+      </c>
+      <c r="L79" t="s">
+        <v>26</v>
+      </c>
+      <c r="P79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" t="s">
+        <v>106</v>
+      </c>
+      <c r="E80" t="s">
+        <v>22</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G80" t="s">
+        <v>24</v>
+      </c>
+      <c r="K80" t="s">
+        <v>25</v>
+      </c>
+      <c r="L80" t="s">
+        <v>26</v>
+      </c>
+      <c r="P80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" t="s">
+        <v>108</v>
+      </c>
+      <c r="E81" t="s">
+        <v>22</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" t="s">
+        <v>24</v>
+      </c>
+      <c r="K81" t="s">
+        <v>25</v>
+      </c>
+      <c r="L81" t="s">
+        <v>26</v>
+      </c>
+      <c r="P81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>96</v>
+      </c>
+      <c r="D82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E82" t="s">
+        <v>22</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K82" t="s">
+        <v>48</v>
+      </c>
+      <c r="P82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" t="s">
+        <v>88</v>
+      </c>
+      <c r="D83" t="s">
+        <v>99</v>
+      </c>
+      <c r="E83" t="s">
+        <v>100</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="K83" t="s">
+        <v>35</v>
+      </c>
+      <c r="L83" t="s">
+        <v>36</v>
+      </c>
+      <c r="P83" t="s">
+        <v>37</v>
+      </c>
+      <c r="R83" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" t="s">
+        <v>92</v>
+      </c>
+      <c r="D84" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" t="s">
+        <v>22</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G84" t="s">
+        <v>24</v>
+      </c>
+      <c r="K84" t="s">
+        <v>25</v>
+      </c>
+      <c r="L84" t="s">
+        <v>26</v>
+      </c>
+      <c r="P84" t="s">
+        <v>27</v>
+      </c>
+      <c r="R84" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" t="s">
+        <v>104</v>
+      </c>
+      <c r="E85" t="s">
+        <v>22</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G85" t="s">
+        <v>24</v>
+      </c>
+      <c r="K85" t="s">
+        <v>25</v>
+      </c>
+      <c r="L85" t="s">
+        <v>26</v>
+      </c>
+      <c r="P85" t="s">
+        <v>27</v>
+      </c>
+      <c r="R85" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" t="s">
+        <v>106</v>
+      </c>
+      <c r="E86" t="s">
+        <v>22</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G86" t="s">
+        <v>24</v>
+      </c>
+      <c r="K86" t="s">
+        <v>25</v>
+      </c>
+      <c r="L86" t="s">
+        <v>26</v>
+      </c>
+      <c r="P86" t="s">
+        <v>27</v>
+      </c>
+      <c r="R86" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87" t="s">
+        <v>22</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G87" t="s">
+        <v>24</v>
+      </c>
+      <c r="K87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L87" t="s">
+        <v>26</v>
+      </c>
+      <c r="P87" t="s">
+        <v>27</v>
+      </c>
+      <c r="R87" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>46</v>
+      </c>
+      <c r="B88" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" t="s">
+        <v>109</v>
+      </c>
+      <c r="E88" t="s">
+        <v>22</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K88" t="s">
+        <v>48</v>
+      </c>
+      <c r="P88" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" t="s">
+        <v>60</v>
+      </c>
+      <c r="C89" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" t="s">
+        <v>22</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" t="s">
+        <v>24</v>
+      </c>
+      <c r="K89" t="s">
+        <v>25</v>
+      </c>
+      <c r="L89" t="s">
+        <v>26</v>
+      </c>
+      <c r="P89" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" t="s">
+        <v>60</v>
+      </c>
+      <c r="C90" t="s">
+        <v>93</v>
+      </c>
+      <c r="D90" t="s">
+        <v>104</v>
+      </c>
+      <c r="E90" t="s">
+        <v>22</v>
+      </c>
+      <c r="F90" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G90" t="s">
+        <v>24</v>
+      </c>
+      <c r="K90" t="s">
+        <v>25</v>
+      </c>
+      <c r="L90" t="s">
+        <v>26</v>
+      </c>
+      <c r="P90" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" t="s">
+        <v>60</v>
+      </c>
+      <c r="C91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D91" t="s">
+        <v>106</v>
+      </c>
+      <c r="E91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G91" t="s">
+        <v>24</v>
+      </c>
+      <c r="K91" t="s">
+        <v>25</v>
+      </c>
+      <c r="L91" t="s">
+        <v>26</v>
+      </c>
+      <c r="P91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" t="s">
+        <v>60</v>
+      </c>
+      <c r="C92" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" t="s">
+        <v>108</v>
+      </c>
+      <c r="E92" t="s">
+        <v>22</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G92" t="s">
+        <v>24</v>
+      </c>
+      <c r="K92" t="s">
+        <v>25</v>
+      </c>
+      <c r="L92" t="s">
+        <v>26</v>
+      </c>
+      <c r="P92" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" t="s">
+        <v>60</v>
+      </c>
+      <c r="C93" t="s">
+        <v>96</v>
+      </c>
+      <c r="D93" t="s">
+        <v>109</v>
+      </c>
+      <c r="E93" t="s">
+        <v>22</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K93" t="s">
+        <v>48</v>
+      </c>
+      <c r="P93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>30</v>
+      </c>
+      <c r="B94" t="s">
+        <v>111</v>
+      </c>
+      <c r="C94" t="s">
+        <v>88</v>
+      </c>
+      <c r="D94" t="s">
+        <v>99</v>
+      </c>
+      <c r="E94" t="s">
+        <v>100</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K94" t="s">
+        <v>35</v>
+      </c>
+      <c r="L94" t="s">
+        <v>36</v>
+      </c>
+      <c r="P94" t="s">
+        <v>37</v>
+      </c>
+      <c r="R94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" t="s">
+        <v>111</v>
+      </c>
+      <c r="C95" t="s">
+        <v>97</v>
+      </c>
+      <c r="D95" t="s">
+        <v>113</v>
+      </c>
+      <c r="E95" t="s">
+        <v>100</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="K95" t="s">
+        <v>35</v>
+      </c>
+      <c r="L95" t="s">
+        <v>36</v>
+      </c>
+      <c r="P95" t="s">
+        <v>37</v>
+      </c>
+      <c r="R95" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" t="s">
+        <v>111</v>
+      </c>
+      <c r="C96" t="s">
+        <v>98</v>
+      </c>
+      <c r="D96" t="s">
+        <v>115</v>
+      </c>
+      <c r="E96" t="s">
+        <v>100</v>
+      </c>
+      <c r="F96" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="K96" t="s">
+        <v>35</v>
+      </c>
+      <c r="L96" t="s">
+        <v>36</v>
+      </c>
+      <c r="P96" t="s">
+        <v>37</v>
+      </c>
+      <c r="R96" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" t="s">
+        <v>111</v>
+      </c>
+      <c r="C97" t="s">
+        <v>90</v>
+      </c>
+      <c r="D97" t="s">
+        <v>104</v>
+      </c>
+      <c r="E97" t="s">
+        <v>100</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="K97" t="s">
+        <v>35</v>
+      </c>
+      <c r="L97" t="s">
+        <v>36</v>
+      </c>
+      <c r="P97" t="s">
+        <v>37</v>
+      </c>
+      <c r="R97" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98" t="s">
+        <v>111</v>
+      </c>
+      <c r="C98" t="s">
+        <v>91</v>
+      </c>
+      <c r="D98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E98" t="s">
+        <v>100</v>
+      </c>
+      <c r="F98" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="K98" t="s">
+        <v>35</v>
+      </c>
+      <c r="L98" t="s">
+        <v>36</v>
+      </c>
+      <c r="P98" t="s">
+        <v>37</v>
+      </c>
+      <c r="R98" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" t="s">
+        <v>111</v>
+      </c>
+      <c r="C99" t="s">
+        <v>92</v>
+      </c>
+      <c r="D99" t="s">
+        <v>107</v>
+      </c>
+      <c r="E99" t="s">
+        <v>22</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G99" t="s">
+        <v>24</v>
+      </c>
+      <c r="K99" t="s">
+        <v>25</v>
+      </c>
+      <c r="L99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P99" t="s">
+        <v>27</v>
+      </c>
+      <c r="R99" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s">
+        <v>111</v>
+      </c>
+      <c r="C100" t="s">
+        <v>93</v>
+      </c>
+      <c r="D100" t="s">
+        <v>104</v>
+      </c>
+      <c r="E100" t="s">
+        <v>22</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G100" t="s">
+        <v>24</v>
+      </c>
+      <c r="K100" t="s">
+        <v>25</v>
+      </c>
+      <c r="L100" t="s">
+        <v>26</v>
+      </c>
+      <c r="P100" t="s">
+        <v>27</v>
+      </c>
+      <c r="R100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" t="s">
+        <v>111</v>
+      </c>
+      <c r="C101" t="s">
+        <v>94</v>
+      </c>
+      <c r="D101" t="s">
+        <v>106</v>
+      </c>
+      <c r="E101" t="s">
+        <v>22</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G101" t="s">
+        <v>24</v>
+      </c>
+      <c r="K101" t="s">
+        <v>25</v>
+      </c>
+      <c r="L101" t="s">
+        <v>26</v>
+      </c>
+      <c r="P101" t="s">
+        <v>27</v>
+      </c>
+      <c r="R101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" t="s">
+        <v>111</v>
+      </c>
+      <c r="C102" t="s">
+        <v>95</v>
+      </c>
+      <c r="D102" t="s">
+        <v>108</v>
+      </c>
+      <c r="E102" t="s">
+        <v>22</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" t="s">
+        <v>24</v>
+      </c>
+      <c r="K102" t="s">
+        <v>25</v>
+      </c>
+      <c r="L102" t="s">
+        <v>26</v>
+      </c>
+      <c r="P102" t="s">
+        <v>27</v>
+      </c>
+      <c r="R102" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" t="s">
+        <v>96</v>
+      </c>
+      <c r="D103" t="s">
+        <v>109</v>
+      </c>
+      <c r="E103" t="s">
+        <v>22</v>
+      </c>
+      <c r="F103" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K103" t="s">
+        <v>48</v>
+      </c>
+      <c r="P103" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" t="s">
+        <v>63</v>
+      </c>
+      <c r="C104" t="s">
+        <v>88</v>
+      </c>
+      <c r="D104" t="s">
+        <v>99</v>
+      </c>
+      <c r="E104" t="s">
+        <v>100</v>
+      </c>
+      <c r="F104" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="K104" t="s">
+        <v>35</v>
+      </c>
+      <c r="L104" t="s">
+        <v>36</v>
+      </c>
+      <c r="P104" t="s">
+        <v>37</v>
+      </c>
+      <c r="R104" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" t="s">
+        <v>97</v>
+      </c>
+      <c r="D105" t="s">
+        <v>113</v>
+      </c>
+      <c r="E105" t="s">
+        <v>100</v>
+      </c>
+      <c r="F105" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="K105" t="s">
+        <v>35</v>
+      </c>
+      <c r="L105" t="s">
+        <v>36</v>
+      </c>
+      <c r="P105" t="s">
+        <v>37</v>
+      </c>
+      <c r="R105" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" t="s">
+        <v>63</v>
+      </c>
+      <c r="C106" t="s">
+        <v>98</v>
+      </c>
+      <c r="D106" t="s">
+        <v>115</v>
+      </c>
+      <c r="E106" t="s">
+        <v>100</v>
+      </c>
+      <c r="F106" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="K106" t="s">
+        <v>35</v>
+      </c>
+      <c r="L106" t="s">
+        <v>36</v>
+      </c>
+      <c r="P106" t="s">
+        <v>37</v>
+      </c>
+      <c r="R106" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" t="s">
+        <v>63</v>
+      </c>
+      <c r="C107" t="s">
+        <v>92</v>
+      </c>
+      <c r="D107" t="s">
+        <v>107</v>
+      </c>
+      <c r="E107" t="s">
+        <v>22</v>
+      </c>
+      <c r="F107" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G107" t="s">
+        <v>24</v>
+      </c>
+      <c r="K107" t="s">
+        <v>25</v>
+      </c>
+      <c r="L107" t="s">
+        <v>26</v>
+      </c>
+      <c r="P107" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" t="s">
+        <v>63</v>
+      </c>
+      <c r="C108" t="s">
+        <v>93</v>
+      </c>
+      <c r="D108" t="s">
+        <v>104</v>
+      </c>
+      <c r="E108" t="s">
+        <v>22</v>
+      </c>
+      <c r="F108" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G108" t="s">
+        <v>24</v>
+      </c>
+      <c r="K108" t="s">
+        <v>25</v>
+      </c>
+      <c r="L108" t="s">
+        <v>26</v>
+      </c>
+      <c r="P108" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" t="s">
+        <v>63</v>
+      </c>
+      <c r="C109" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" t="s">
+        <v>106</v>
+      </c>
+      <c r="E109" t="s">
+        <v>22</v>
+      </c>
+      <c r="F109" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G109" t="s">
+        <v>24</v>
+      </c>
+      <c r="K109" t="s">
+        <v>25</v>
+      </c>
+      <c r="L109" t="s">
+        <v>26</v>
+      </c>
+      <c r="P109" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" t="s">
+        <v>63</v>
+      </c>
+      <c r="C110" t="s">
+        <v>95</v>
+      </c>
+      <c r="D110" t="s">
+        <v>108</v>
+      </c>
+      <c r="E110" t="s">
+        <v>22</v>
+      </c>
+      <c r="F110" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G110" t="s">
+        <v>24</v>
+      </c>
+      <c r="K110" t="s">
+        <v>25</v>
+      </c>
+      <c r="L110" t="s">
+        <v>26</v>
+      </c>
+      <c r="P110" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>46</v>
+      </c>
+      <c r="B111" t="s">
+        <v>63</v>
+      </c>
+      <c r="C111" t="s">
+        <v>96</v>
+      </c>
+      <c r="D111" t="s">
+        <v>109</v>
+      </c>
+      <c r="E111" t="s">
+        <v>22</v>
+      </c>
+      <c r="F111" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K111" t="s">
+        <v>48</v>
+      </c>
+      <c r="P111" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>30</v>
+      </c>
+      <c r="B112" t="s">
+        <v>68</v>
+      </c>
+      <c r="C112" t="s">
+        <v>88</v>
+      </c>
+      <c r="D112" t="s">
+        <v>99</v>
+      </c>
+      <c r="E112" t="s">
+        <v>100</v>
+      </c>
+      <c r="F112" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="K112" t="s">
+        <v>35</v>
+      </c>
+      <c r="L112" t="s">
+        <v>36</v>
+      </c>
+      <c r="P112" t="s">
+        <v>37</v>
+      </c>
+      <c r="R112" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" t="s">
+        <v>97</v>
+      </c>
+      <c r="D113" t="s">
+        <v>113</v>
+      </c>
+      <c r="E113" t="s">
+        <v>100</v>
+      </c>
+      <c r="F113" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="K113" t="s">
+        <v>35</v>
+      </c>
+      <c r="L113" t="s">
+        <v>36</v>
+      </c>
+      <c r="P113" t="s">
+        <v>37</v>
+      </c>
+      <c r="R113" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" t="s">
+        <v>98</v>
+      </c>
+      <c r="D114" t="s">
+        <v>115</v>
+      </c>
+      <c r="E114" t="s">
+        <v>100</v>
+      </c>
+      <c r="F114" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="K114" t="s">
+        <v>35</v>
+      </c>
+      <c r="L114" t="s">
+        <v>36</v>
+      </c>
+      <c r="P114" t="s">
+        <v>37</v>
+      </c>
+      <c r="R114" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" t="s">
+        <v>92</v>
+      </c>
+      <c r="D115" t="s">
+        <v>107</v>
+      </c>
+      <c r="E115" t="s">
+        <v>22</v>
+      </c>
+      <c r="F115" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G115" t="s">
+        <v>24</v>
+      </c>
+      <c r="K115" t="s">
+        <v>25</v>
+      </c>
+      <c r="L115" t="s">
+        <v>26</v>
+      </c>
+      <c r="P115" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" t="s">
+        <v>93</v>
+      </c>
+      <c r="D116" t="s">
+        <v>104</v>
+      </c>
+      <c r="E116" t="s">
+        <v>22</v>
+      </c>
+      <c r="F116" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G116" t="s">
+        <v>24</v>
+      </c>
+      <c r="K116" t="s">
+        <v>25</v>
+      </c>
+      <c r="L116" t="s">
+        <v>26</v>
+      </c>
+      <c r="P116" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" t="s">
+        <v>68</v>
+      </c>
+      <c r="C117" t="s">
+        <v>94</v>
+      </c>
+      <c r="D117" t="s">
+        <v>106</v>
+      </c>
+      <c r="E117" t="s">
+        <v>22</v>
+      </c>
+      <c r="F117" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G117" t="s">
+        <v>24</v>
+      </c>
+      <c r="K117" t="s">
+        <v>25</v>
+      </c>
+      <c r="L117" t="s">
+        <v>26</v>
+      </c>
+      <c r="P117" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" t="s">
+        <v>68</v>
+      </c>
+      <c r="C118" t="s">
+        <v>95</v>
+      </c>
+      <c r="D118" t="s">
+        <v>108</v>
+      </c>
+      <c r="E118" t="s">
+        <v>22</v>
+      </c>
+      <c r="F118" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G118" t="s">
+        <v>24</v>
+      </c>
+      <c r="K118" t="s">
+        <v>25</v>
+      </c>
+      <c r="L118" t="s">
+        <v>26</v>
+      </c>
+      <c r="P118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>46</v>
+      </c>
+      <c r="B119" t="s">
+        <v>68</v>
+      </c>
+      <c r="C119" t="s">
+        <v>96</v>
+      </c>
+      <c r="D119" t="s">
+        <v>109</v>
+      </c>
+      <c r="E119" t="s">
+        <v>22</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K119" t="s">
+        <v>48</v>
+      </c>
+      <c r="P119" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:R73" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="C51:D51"/>

</xml_diff>